<commit_message>
Revision y modificacion varios
</commit_message>
<xml_diff>
--- a/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
+++ b/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mramirez\source\repos\PLANILLACONTABLE\INFORME\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\source\repos\lctsistemas\PLANILLACONTABLE\INFORME\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C91D36E-FCA2-42AA-9ECC-41591E17E472}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D32CF0-5A5C-4106-9E25-54AAF17579D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FCCD8F72-B774-436A-AA0E-7E24570ECBB1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{FCCD8F72-B774-436A-AA0E-7E24570ECBB1}"/>
   </bookViews>
   <sheets>
     <sheet name="INFORMES" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>INFORME DE  DESARROLLO DE SITEMA PLANILLA LCT.</t>
   </si>
@@ -106,25 +106,43 @@
     <t xml:space="preserve">Listar empleados de la misma empresa una vez que se logueen </t>
   </si>
   <si>
-    <r>
-      <t>revisar codigo empresa, para que se registre uno solo(crear condicion)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>pendiente</t>
-    </r>
-  </si>
-  <si>
     <t>Revisar contrato para que salga el boton modificar una vez que se registra un contrato</t>
   </si>
   <si>
-    <t>tabla empresa</t>
+    <t xml:space="preserve">GESTION EMPLEADO(registrar, actualizar mostrar y eliminar) mediante procedimientos alamacenados </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GESTION DE BANCO(registrar, actualizar mostrar y eliminar) mediante procedimientos alamacenados </t>
+  </si>
+  <si>
+    <t>Revisando lista de empleados por empresa una vez que se logueen</t>
+  </si>
+  <si>
+    <t>Modificar Diseño de empleado,  banco y tipo de contrato</t>
+  </si>
+  <si>
+    <t>Verificando Errores, corregir Sucursal(no actualiza), modificar proc sql de empleado y sincronizar datos con empresa y empleado individual ok</t>
+  </si>
+  <si>
+    <t>Modificacion del Diseño de empresa y Sucursal(para registrar empleado por empresa).</t>
+  </si>
+  <si>
+    <t>9 pm a 2 am</t>
+  </si>
+  <si>
+    <t>OBSERVACION</t>
+  </si>
+  <si>
+    <t>PENDIENTE</t>
+  </si>
+  <si>
+    <t>CONCLUIDO</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>revisar codigo empresa, para que se registre uno solo(crear condicion)</t>
   </si>
   <si>
     <r>
@@ -138,23 +156,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> pendiente</t>
+      <t xml:space="preserve"> </t>
     </r>
   </si>
   <si>
-    <t>Verificando Errores, corregir Sucursal(no actualiza)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GESTION EMPLEADO(registrar, actualizar mostrar y eliminar) mediante procedimientos alamacenados </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GESTION DE BANCO(registrar, actualizar mostrar y eliminar) mediante procedimientos alamacenados </t>
-  </si>
-  <si>
-    <t>Revisando lista de empleados por empresa una vez que se logueen</t>
-  </si>
-  <si>
-    <t>Modificar Diseño de empleado,  banco y tipo de contrato</t>
+    <t>Crear formulario Principal(contenedor de formularios)</t>
+  </si>
+  <si>
+    <t>Crear base de datos (tabla periodo)</t>
+  </si>
+  <si>
+    <t>Crear procedimiento sql para buscar empleado</t>
   </si>
 </sst>
 </file>
@@ -164,7 +176,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,6 +220,45 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -229,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -263,11 +314,54 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FFFF0000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -300,7 +394,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0B75897D-100D-4D5D-A86B-35010016B1AC}" name="Tabla2" displayName="Tabla2" ref="A10:I16" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0B75897D-100D-4D5D-A86B-35010016B1AC}" name="Tabla2" displayName="Tabla2" ref="A10:I16" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A10:I16" xr:uid="{6365733F-180E-4727-A920-FF2F299610E8}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{5F4B84F2-079F-4219-8B8A-49571F8DD414}" name="OTRO"/>
@@ -312,6 +406,17 @@
     <tableColumn id="7" xr3:uid="{F0FFB24A-3EC5-4950-94CE-AD109E600912}" name="SÁBADO"/>
     <tableColumn id="8" xr3:uid="{99DDF987-B514-45B9-BD41-25FA55BB12B7}" name="DOMINGO"/>
     <tableColumn id="9" xr3:uid="{B5C2F3B1-9610-4987-8C53-CCEFF66905A8}" name="DEVELOPER"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{04AD6298-28CB-428C-BC07-9A916C01371B}" name="Tabla1" displayName="Tabla1" ref="A2:C9" totalsRowShown="0">
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{E9815E11-92DB-4879-9FCB-B1A5500BE9A2}" name="OBSERVACION"/>
+    <tableColumn id="2" xr3:uid="{902F1039-067B-4EC4-8EC7-F6CB2D6E8B95}" name="PENDIENTE" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{7FDB06FA-8703-4553-A95A-D6CC27A41B6C}" name="CONCLUIDO" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -616,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55C9F99B-5DD8-4619-A25C-4AB7EC88545F}">
   <dimension ref="A2:I17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A11" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A8" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,7 +730,7 @@
     <col min="1" max="1" width="15.140625" customWidth="1"/>
     <col min="2" max="2" width="17.140625" customWidth="1"/>
     <col min="3" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" customWidth="1"/>
     <col min="6" max="8" width="15.140625" customWidth="1"/>
     <col min="9" max="9" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -727,12 +832,14 @@
         <v>16</v>
       </c>
       <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+      <c r="F12" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
@@ -743,9 +850,11 @@
         <v>14</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="10" t="s">
@@ -790,16 +899,16 @@
     </row>
     <row r="16" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -820,7 +929,7 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="59" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="57" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -829,47 +938,94 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB2E3E90-1FAF-4E03-9CF4-0E6F2FB5F484}">
-  <dimension ref="A3:A12"/>
+  <dimension ref="A2:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView view="pageBreakPreview" zoomScale="145" zoomScaleNormal="100" zoomScaleSheetLayoutView="145" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="78" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="19"/>
+    <col min="3" max="3" width="13.5703125" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5" s="19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
+        <v>38</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="86" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Creacion y relacion de tablas
</commit_message>
<xml_diff>
--- a/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
+++ b/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\source\repos\lctsistemas\PLANILLACONTABLE\INFORME\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mramirez\source\repos\PLANILLACONTABLE\INFORME\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{707281D1-339F-44A1-8D2A-EC50D6AAB975}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE45E5B-97BF-49A8-B54C-6B19F42BC794}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="726" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="726" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INFORME" sheetId="4" r:id="rId1"/>
     <sheet name="PENDIENTES" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja1" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="63">
   <si>
     <t>INFORME DE  DESARROLLO DE SITEMA PLANILLA LCT.</t>
   </si>
@@ -195,6 +195,39 @@
   </si>
   <si>
     <t>Modificar procedimiento SP_REMOVE_SUCURSAL(para eliminar empresa y sucursal)</t>
+  </si>
+  <si>
+    <t>gratificacion manto</t>
+  </si>
+  <si>
+    <t>cts</t>
+  </si>
+  <si>
+    <t>cts manto</t>
+  </si>
+  <si>
+    <t>planilla</t>
+  </si>
+  <si>
+    <t>periodo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">crear tabla agregar meses </t>
+  </si>
+  <si>
+    <t>tabla abstracta</t>
+  </si>
+  <si>
+    <t>Crear tabla gratificacion</t>
+  </si>
+  <si>
+    <t>JUAN FLORES/ANDRE ACEDO</t>
+  </si>
+  <si>
+    <t>Crear tablas para realizar los respectivos calculos de la planilla  y realizar las conexiones correspondientes con la base de datos del sistema.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diseño y creacion del formulario principal al momento que el usuario inicie sesion con su empresa. </t>
   </si>
 </sst>
 </file>
@@ -483,8 +516,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{209129E8-390A-49F0-9FAE-2E6BC4E8FC93}" name="Tabla3" displayName="Tabla3" ref="A10:H20" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A10:H20" xr:uid="{CE052CFC-4D65-4396-BD5D-008CF3C6222D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{209129E8-390A-49F0-9FAE-2E6BC4E8FC93}" name="Tabla3" displayName="Tabla3" ref="A10:H22" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A10:H22" xr:uid="{CE052CFC-4D65-4396-BD5D-008CF3C6222D}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{FD0E33B8-7E55-42BD-A8FA-A3550E75FA05}" name="LUNES"/>
     <tableColumn id="2" xr3:uid="{245FBD3C-8A65-45EE-BFC1-272B48328239}" name="MARTES"/>
@@ -500,7 +533,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabla1" displayName="Tabla1" ref="A2:D15" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabla1" displayName="Tabla1" ref="A2:D23" totalsRowShown="0">
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="OBSERVACION"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="PENDIENTE" dataDxfId="2"/>
@@ -808,10 +841,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75921E90-C2FD-43C6-ACC7-A767964A2064}">
-  <dimension ref="A2:H21"/>
+  <dimension ref="A2:H22"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A19" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1058,10 +1091,25 @@
         <v>44059</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="D22" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="55" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="51" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -1070,10 +1118,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:E15"/>
+  <dimension ref="A2:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="145" zoomScaleNormal="100" zoomScaleSheetLayoutView="145" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A13" zoomScale="145" zoomScaleNormal="100" zoomScaleSheetLayoutView="145" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1229,6 +1277,62 @@
       <c r="D15" s="15" t="s">
         <v>38</v>
       </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="10"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="10"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="10"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="10"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="10"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="10"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="10"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Edit Design View company and user
</commit_message>
<xml_diff>
--- a/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
+++ b/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\source\repos\lctsistemas\PLANILLACONTABLE\INFORME\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED1811F-E07D-4D90-A08C-0AE28523514A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF25D39-9B73-418A-A683-956543AB09A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="726" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -844,7 +844,7 @@
   <dimension ref="A2:H21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1111,8 +1111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:E20"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A10" zoomScale="145" zoomScaleNormal="100" zoomScaleSheetLayoutView="145" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A13" zoomScale="145" zoomScaleNormal="100" zoomScaleSheetLayoutView="145" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Validacion de datos y diseño form
</commit_message>
<xml_diff>
--- a/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
+++ b/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\source\repos\lctsistemas\PLANILLACONTABLE\INFORME\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124DDF15-F8EB-476D-BFA6-2F6D8B606A92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6179149B-1ED6-4E3D-9A78-4758196E5DA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="726" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="726" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INFORME" sheetId="4" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="70">
   <si>
     <t>INFORME DE  DESARROLLO DE SITEMA PLANILLA LCT.</t>
   </si>
@@ -258,6 +258,12 @@
   </si>
   <si>
     <t>Cambiar diseño de botones de los formularios en C#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login Acceso (error corregido), (Modificar relaciones en Diagrama de clases(DE LA DB) </t>
+  </si>
+  <si>
+    <t>Cambio de diseño(formulario Usuario) Modelo para todos los formulario, Cambiar Filtro para buscar registro e implementar un nuevo componente(DataAnnotations)para validar datos.</t>
   </si>
 </sst>
 </file>
@@ -889,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:H24"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A22" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A22" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1198,12 +1204,18 @@
         <v>44066</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>58</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="H24" s="17" t="s">
         <v>16</v>
@@ -1222,7 +1234,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScale="145" zoomScaleNormal="100" zoomScaleSheetLayoutView="145" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A16" zoomScale="145" zoomScaleNormal="100" zoomScaleSheetLayoutView="145" workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Validacion de registro empresa, usuario, view empresa y cambio en sp_empresa
</commit_message>
<xml_diff>
--- a/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
+++ b/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\source\repos\lctsistemas\PLANILLACONTABLE\INFORME\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6179149B-1ED6-4E3D-9A78-4758196E5DA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18BC8BB7-1CC4-4266-B110-319C61F49D1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="726" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="726" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INFORME" sheetId="4" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="72">
   <si>
     <t>INFORME DE  DESARROLLO DE SITEMA PLANILLA LCT.</t>
   </si>
@@ -260,17 +260,67 @@
     <t>Cambiar diseño de botones de los formularios en C#</t>
   </si>
   <si>
-    <t xml:space="preserve">Login Acceso (error corregido), (Modificar relaciones en Diagrama de clases(DE LA DB) </t>
-  </si>
-  <si>
-    <t>Cambio de diseño(formulario Usuario) Modelo para todos los formulario, Cambiar Filtro para buscar registro e implementar un nuevo componente(DataAnnotations)para validar datos.</t>
+    <t xml:space="preserve">Login Acceso (error corregido), (Modificar relaciones en Diagrama de clases(DE LA BASE DE DATOS) </t>
+  </si>
+  <si>
+    <r>
+      <t>Cambio de diseño(formulario Usuario) Modelo para todos los formulario, Cambiar Filtro para buscar registro e implementar un nuevo componente(DataAnnotations)para validar datos.(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pendiente</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Formulario Usuario en C#(prueba de validacion y filtro al registro)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>concluido</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Formulario Empresa y vista empresa en  C#(validacion y filtro), se modifico el PROCEDIENTO ALMACENADO EN LA DB.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -363,6 +413,20 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -895,8 +959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:H24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A22" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A25" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1217,6 +1281,12 @@
       <c r="D24" s="1" t="s">
         <v>69</v>
       </c>
+      <c r="E24" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="H24" s="17" t="s">
         <v>16</v>
       </c>
@@ -1234,8 +1304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:E23"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A16" zoomScale="145" zoomScaleNormal="100" zoomScaleSheetLayoutView="145" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScale="145" zoomScaleNormal="100" zoomScaleSheetLayoutView="145" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Regimen Update y Delete
</commit_message>
<xml_diff>
--- a/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
+++ b/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\source\repos\lctsistemas\PLANILLACONTABLE\INFORME\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mramirez\source\repos\PLANILLACONTABLE\INFORME\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7686EFA-0F4D-4850-9D3B-BF075D8B03F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B43A2D5-03B7-44F7-923B-A217CD9964E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="726" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="726" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INFORME" sheetId="4" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Hoja1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">INFORME!$A$1:$H$23</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">INFORME!$A$1:$H$26</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="85">
   <si>
     <t>INFORME DE  DESARROLLO DE SITEMA PLANILLA LCT.</t>
   </si>
@@ -347,6 +347,12 @@
   </si>
   <si>
     <t>Formulario Empresa y vista empresa en  C#(validacion y filtro), se modifico el PROCEDIENTO ALMACENADO EN LA DB.</t>
+  </si>
+  <si>
+    <t>Formulario para ingresar un nuevo regimen y conexión con la base de datos mediante un procedimiento almacenado.</t>
+  </si>
+  <si>
+    <t>Formulario para listar los regimenes existentes y conexión con la base de datos mediante un procedimiento almacenado sp_show_regimen.</t>
   </si>
 </sst>
 </file>
@@ -467,12 +473,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -496,7 +508,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -565,12 +577,39 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -601,20 +640,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -685,7 +710,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla3" displayName="Tabla3" ref="A10:H23" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla3" displayName="Tabla3" ref="A10:H23" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A10:H23" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="LUNES"/>
@@ -705,9 +730,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabla1" displayName="Tabla1" ref="A2:D29" totalsRowShown="0">
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="OBSERVACION"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="PENDIENTE" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="CONCLUIDO" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="ENCARGADO" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="PENDIENTE" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="CONCLUIDO" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="ENCARGADO" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1010,10 +1035,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:H23"/>
+  <dimension ref="A2:H26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A22" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A23" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1337,6 +1362,55 @@
         <v>15</v>
       </c>
     </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="25"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="H24" s="17"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="12">
+        <v>44067</v>
+      </c>
+      <c r="B25" s="12">
+        <v>44068</v>
+      </c>
+      <c r="C25" s="12">
+        <v>44069</v>
+      </c>
+      <c r="D25" s="12">
+        <v>44070</v>
+      </c>
+      <c r="E25" s="12">
+        <v>44071</v>
+      </c>
+      <c r="F25" s="12">
+        <v>44072</v>
+      </c>
+      <c r="G25" s="12">
+        <v>44073</v>
+      </c>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A26" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" s="27"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="27" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="51" orientation="portrait" r:id="rId1"/>
@@ -1350,8 +1424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:E29"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A25" zoomScale="145" zoomScaleNormal="100" zoomScaleSheetLayoutView="145" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScale="145" zoomScaleNormal="100" zoomScaleSheetLayoutView="145" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1580,7 +1654,7 @@
       <c r="A21" t="s">
         <v>65</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="C21" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D21" s="15" t="s">

</xml_diff>

<commit_message>
Tipo Contrato y Planilla
</commit_message>
<xml_diff>
--- a/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
+++ b/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mramirez\source\repos\PLANILLACONTABLE\INFORME\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B43A2D5-03B7-44F7-923B-A217CD9964E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66AA39A0-2A1F-4D1C-B5C8-4B61CEAE55D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="726" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="85">
   <si>
     <t>INFORME DE  DESARROLLO DE SITEMA PLANILLA LCT.</t>
   </si>
@@ -359,7 +359,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -472,6 +472,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -508,7 +515,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -590,26 +597,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -640,6 +636,20 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -710,7 +720,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla3" displayName="Tabla3" ref="A10:H23" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla3" displayName="Tabla3" ref="A10:H23" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A10:H23" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="LUNES"/>
@@ -730,9 +740,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabla1" displayName="Tabla1" ref="A2:D29" totalsRowShown="0">
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="OBSERVACION"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="PENDIENTE" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="CONCLUIDO" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="ENCARGADO" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="PENDIENTE" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="CONCLUIDO" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="ENCARGADO" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1425,7 +1435,7 @@
   <dimension ref="A2:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScale="145" zoomScaleNormal="100" zoomScaleSheetLayoutView="145" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1643,7 +1653,8 @@
       <c r="A20" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="32"/>
+      <c r="C20" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D20" s="15" t="s">
@@ -1687,7 +1698,7 @@
       <c r="A24" t="s">
         <v>68</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="C24" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D24" s="15" t="s">
@@ -1723,6 +1734,9 @@
       <c r="B27" s="7" t="s">
         <v>29</v>
       </c>
+      <c r="C27" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="D27" s="15" t="s">
         <v>75</v>
       </c>
@@ -1732,6 +1746,9 @@
         <v>73</v>
       </c>
       <c r="B28" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D28" s="15" t="s">

</xml_diff>

<commit_message>
script empleado, contrato, comisiones
</commit_message>
<xml_diff>
--- a/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
+++ b/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\source\repos\lctsistemas\PLANILLACONTABLE\INFORME\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7686EFA-0F4D-4850-9D3B-BF075D8B03F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DDF318-B397-4F0C-A8A4-D28D980FE88F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="726" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,9 +18,9 @@
     <sheet name="Hoja1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">INFORME!$A$1:$H$23</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">INFORME!$A$1:$H$25</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="85">
   <si>
     <t>INFORME DE  DESARROLLO DE SITEMA PLANILLA LCT.</t>
   </si>
@@ -347,6 +347,12 @@
   </si>
   <si>
     <t>Formulario Empresa y vista empresa en  C#(validacion y filtro), se modifico el PROCEDIENTO ALMACENADO EN LA DB.</t>
+  </si>
+  <si>
+    <t>Formulario Sucursal, vista usuario en C#(validacion y filtro), se modifico el procedimiento almacenado en la DB.</t>
+  </si>
+  <si>
+    <t>Tablas empleado, contrato, comisiones(modificado) y alterar los procedimientos almacenados de las tablas en sqlserver</t>
   </si>
 </sst>
 </file>
@@ -475,7 +481,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -483,20 +489,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -561,9 +558,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -571,6 +565,20 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -601,20 +609,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -685,8 +679,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla3" displayName="Tabla3" ref="A10:H23" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A10:H23" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla3" displayName="Tabla3" ref="A10:H25" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A10:H25" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="LUNES"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="MARTES"/>
@@ -705,9 +699,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabla1" displayName="Tabla1" ref="A2:D29" totalsRowShown="0">
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="OBSERVACION"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="PENDIENTE" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="CONCLUIDO" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="ENCARGADO" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="PENDIENTE" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="CONCLUIDO" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="ENCARGADO" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1010,10 +1004,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:H23"/>
+  <dimension ref="A2:H25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A22" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1315,25 +1309,59 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="150" x14ac:dyDescent="0.25">
-      <c r="A23" s="26" t="s">
+      <c r="A23" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="26" t="s">
+      <c r="B23" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="D23" s="26" t="s">
+      <c r="D23" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="E23" s="26" t="s">
+      <c r="E23" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="F23" s="26" t="s">
+      <c r="F23" s="25" t="s">
         <v>82</v>
       </c>
       <c r="H23" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="12">
+        <v>44067</v>
+      </c>
+      <c r="B24" s="12">
+        <v>44068</v>
+      </c>
+      <c r="C24" s="12">
+        <v>44069</v>
+      </c>
+      <c r="D24" s="12">
+        <v>44070</v>
+      </c>
+      <c r="E24" s="12">
+        <v>44071</v>
+      </c>
+      <c r="F24" s="12">
+        <v>44072</v>
+      </c>
+      <c r="G24" s="12">
+        <v>44073</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="C25" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="H25" s="17" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1350,8 +1378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:E29"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A25" zoomScale="145" zoomScaleNormal="100" zoomScaleSheetLayoutView="145" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A19" zoomScale="145" zoomScaleNormal="100" zoomScaleSheetLayoutView="145" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1572,6 +1600,9 @@
       <c r="B20" s="7" t="s">
         <v>29</v>
       </c>
+      <c r="C20" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="D20" s="15" t="s">
         <v>37</v>
       </c>
@@ -1635,7 +1666,7 @@
       <c r="A26" t="s">
         <v>71</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="C26" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D26" s="15" t="s">

</xml_diff>

<commit_message>
Empleado y contrato en  SqlServer y C#
</commit_message>
<xml_diff>
--- a/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
+++ b/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\source\repos\lctsistemas\PLANILLACONTABLE\INFORME\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DDF318-B397-4F0C-A8A4-D28D980FE88F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED9A9E30-A9CF-46D5-88DB-D1CA03FDD566}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="726" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Hoja1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">INFORME!$A$1:$H$25</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">INFORME!$A$1:$H$24</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="86">
   <si>
     <t>INFORME DE  DESARROLLO DE SITEMA PLANILLA LCT.</t>
   </si>
@@ -174,9 +174,6 @@
   </si>
   <si>
     <t>LOGIN ACCESO(sincronizar con la base de datos)</t>
-  </si>
-  <si>
-    <t>HORA</t>
   </si>
   <si>
     <t>Modificar procedimiento almacenado para preparar scrip en sql transact(para empresa y sucursal, codigo unico y no duplicado)</t>
@@ -353,6 +350,12 @@
   </si>
   <si>
     <t>Tablas empleado, contrato, comisiones(modificado) y alterar los procedimientos almacenados de las tablas en sqlserver</t>
+  </si>
+  <si>
+    <t>Tabla contrato Modificado(en sqlserver), Diseño de empleado y su contrato en C# e insertar datos a la lista desplegable para mostrar información.  Crear sus respectivos procedimientos almacenados en sqlserver.</t>
+  </si>
+  <si>
+    <t>Analis Diagrama de Base de datos, cambios en la realación de tablas(cardinalidad)</t>
   </si>
 </sst>
 </file>
@@ -493,7 +496,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -542,9 +545,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -565,20 +565,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -609,6 +595,20 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -679,8 +679,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla3" displayName="Tabla3" ref="A10:H25" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A10:H25" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla3" displayName="Tabla3" ref="A10:H24" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A10:H24" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="LUNES"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="MARTES"/>
@@ -699,9 +699,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabla1" displayName="Tabla1" ref="A2:D29" totalsRowShown="0">
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="OBSERVACION"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="PENDIENTE" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="CONCLUIDO" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="ENCARGADO" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="PENDIENTE" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="CONCLUIDO" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="ENCARGADO" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1004,15 +1004,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:H25"/>
+  <dimension ref="A2:H24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A22" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24" customWidth="1"/>
     <col min="2" max="2" width="21.140625" customWidth="1"/>
     <col min="3" max="3" width="20.85546875" customWidth="1"/>
     <col min="4" max="4" width="23.28515625" customWidth="1"/>
@@ -1189,13 +1189,13 @@
     </row>
     <row r="16" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="D16" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H16" s="17" t="s">
         <v>15</v>
@@ -1224,150 +1224,151 @@
         <v>44059</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" s="11" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="D19" s="18" t="s">
+    <row r="18" spans="1:8" s="11" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="D18" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="H18" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="E19" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="F19" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="H19" s="18" t="s">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="12">
+        <v>44060</v>
+      </c>
+      <c r="B19" s="12">
+        <v>44061</v>
+      </c>
+      <c r="C19" s="12">
+        <v>44062</v>
+      </c>
+      <c r="D19" s="12">
+        <v>44063</v>
+      </c>
+      <c r="E19" s="12">
+        <v>44064</v>
+      </c>
+      <c r="F19" s="12">
+        <v>44065</v>
+      </c>
+      <c r="G19" s="12">
+        <v>44066</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+      <c r="B20" s="20" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="12">
+      <c r="C20" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="19"/>
+      <c r="E20" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="F20" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="G20" s="19"/>
+      <c r="H20" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="12">
         <v>44060</v>
       </c>
-      <c r="B20" s="12">
+      <c r="B21" s="12">
         <v>44061</v>
       </c>
-      <c r="C20" s="12">
+      <c r="C21" s="12">
         <v>44062</v>
       </c>
-      <c r="D20" s="12">
+      <c r="D21" s="12">
         <v>44063</v>
       </c>
-      <c r="E20" s="12">
+      <c r="E21" s="12">
         <v>44064</v>
       </c>
-      <c r="F20" s="12">
+      <c r="F21" s="12">
         <v>44065</v>
       </c>
-      <c r="G20" s="12">
+      <c r="G21" s="12">
         <v>44066</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="135" x14ac:dyDescent="0.25">
-      <c r="B21" s="21" t="s">
+    <row r="22" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+      <c r="A22" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D21" s="20"/>
-      <c r="E21" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="F21" s="25" t="s">
+      <c r="B22" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="G21" s="20"/>
-      <c r="H21" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="12">
-        <v>44060</v>
-      </c>
-      <c r="B22" s="12">
-        <v>44061</v>
-      </c>
-      <c r="C22" s="12">
-        <v>44062</v>
-      </c>
-      <c r="D22" s="12">
-        <v>44063</v>
-      </c>
-      <c r="E22" s="12">
-        <v>44064</v>
-      </c>
-      <c r="F22" s="12">
-        <v>44065</v>
-      </c>
-      <c r="G22" s="12">
-        <v>44066</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="150" x14ac:dyDescent="0.25">
-      <c r="A23" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="B23" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="C23" s="25" t="s">
+      <c r="D22" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="D23" s="25" t="s">
+      <c r="E22" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="E23" s="25" t="s">
+      <c r="F22" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="F23" s="25" t="s">
+      <c r="H22" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="12">
+        <v>44067</v>
+      </c>
+      <c r="B23" s="12">
+        <v>44068</v>
+      </c>
+      <c r="C23" s="12">
+        <v>44069</v>
+      </c>
+      <c r="D23" s="12">
+        <v>44070</v>
+      </c>
+      <c r="E23" s="12">
+        <v>44071</v>
+      </c>
+      <c r="F23" s="12">
+        <v>44072</v>
+      </c>
+      <c r="G23" s="12">
+        <v>44073</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H23" s="17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="12">
-        <v>44067</v>
-      </c>
-      <c r="B24" s="12">
-        <v>44068</v>
-      </c>
-      <c r="C24" s="12">
-        <v>44069</v>
-      </c>
-      <c r="D24" s="12">
-        <v>44070</v>
-      </c>
-      <c r="E24" s="12">
-        <v>44071</v>
-      </c>
-      <c r="F24" s="12">
-        <v>44072</v>
-      </c>
-      <c r="G24" s="12">
-        <v>44073</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="C25" s="1" t="s">
+      <c r="D24" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="D25" s="23" t="s">
+      <c r="E24" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="H25" s="17" t="s">
+      <c r="H24" s="17" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="51" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="50" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -1378,7 +1379,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:E29"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A19" zoomScale="145" zoomScaleNormal="100" zoomScaleSheetLayoutView="145" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A28" zoomScale="145" zoomScaleNormal="100" zoomScaleSheetLayoutView="145" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -1483,7 +1484,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>29</v>
@@ -1500,23 +1501,23 @@
         <v>29</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>62</v>
-      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
-        <v>60</v>
+      <c r="A13" s="21" t="s">
+        <v>59</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>29</v>
@@ -1539,7 +1540,7 @@
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>29</v>
@@ -1550,7 +1551,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>29</v>
@@ -1561,7 +1562,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>29</v>
@@ -1572,7 +1573,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>29</v>
@@ -1583,19 +1584,19 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="22" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="23" t="s">
-        <v>63</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>29</v>
@@ -1609,7 +1610,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>29</v>
@@ -1620,7 +1621,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>29</v>
@@ -1631,7 +1632,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>29</v>
@@ -1642,18 +1643,18 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="15" t="s">
         <v>68</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>29</v>
@@ -1664,7 +1665,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>29</v>
@@ -1675,35 +1676,35 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="15" t="s">
         <v>74</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
script sql y diseño en C# empleado y contrato
</commit_message>
<xml_diff>
--- a/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
+++ b/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\source\repos\lctsistemas\PLANILLACONTABLE\INFORME\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED9A9E30-A9CF-46D5-88DB-D1CA03FDD566}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{556DF9B8-53C7-46E7-8C3A-345BA30DC607}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="726" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="726" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INFORME" sheetId="4" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="87">
   <si>
     <t>INFORME DE  DESARROLLO DE SITEMA PLANILLA LCT.</t>
   </si>
@@ -356,6 +356,9 @@
   </si>
   <si>
     <t>Analis Diagrama de Base de datos, cambios en la realación de tablas(cardinalidad)</t>
+  </si>
+  <si>
+    <t>Modificar Procedimiento mostrar en sqlserver(banco, tipo documento, cargo, tipo de contrato) se borro varias lineas de codigo en sqlserver y C#</t>
   </si>
 </sst>
 </file>
@@ -1006,8 +1009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:H24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A22" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A22" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1362,6 +1365,9 @@
       <c r="E24" s="1" t="s">
         <v>84</v>
       </c>
+      <c r="F24" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="H24" s="17" t="s">
         <v>15</v>
       </c>
@@ -1379,8 +1385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:E29"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A28" zoomScale="145" zoomScaleNormal="100" zoomScaleSheetLayoutView="145" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="145" zoomScaleNormal="100" zoomScaleSheetLayoutView="145" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1645,7 +1651,7 @@
       <c r="A24" t="s">
         <v>67</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="C24" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D24" s="15" t="s">

</xml_diff>

<commit_message>
DATAROW para mostrar datos laborales del empleado
</commit_message>
<xml_diff>
--- a/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
+++ b/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\source\repos\lctsistemas\PLANILLACONTABLE\INFORME\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27FEBAE-02C0-4AF6-B36B-5F8421ABE6B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E5FC030-CF93-4CE6-9EFE-958BB5636B1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="726" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="INFORME" sheetId="4" r:id="rId1"/>
-    <sheet name="PENDIENTES" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja1" sheetId="3" r:id="rId3"/>
+    <sheet name="INFORME AGOSTO" sheetId="4" r:id="rId1"/>
+    <sheet name="INFORME SEPTIEMBRE" sheetId="5" r:id="rId2"/>
+    <sheet name="PENDIENTES" sheetId="2" r:id="rId3"/>
+    <sheet name="Hoja1" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">INFORME!$A$1:$H$27</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'INFORME AGOSTO'!$A$1:$H$27</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="96">
   <si>
     <t>INFORME DE  DESARROLLO DE SITEMA PLANILLA LCT.</t>
   </si>
@@ -400,12 +401,95 @@
   <si>
     <t>Modificar Procedimiento mostrar en sqlserver(banco, tipo documento, cargo, tipo de contrato) se borro varias lineas de codigo en sqlserver y C#</t>
   </si>
+  <si>
+    <t>Se inserto datos a la tabla Empleado y contrato (con un solo proceso)para eso, se modifico los procedimientos en SQLSERVER Y el codigo fuente en VBC#</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Listar solo Nombre de empleado al ser registrado y contratado, luego se tendra que mostrar todos sus datos laborales en los campos del formulario para su respectiva Actualizacion( </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pendiente</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>en</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pruebas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Se hizo varias pruebas(para mostrar datos laborales en campos del formulario), en conclucion se implemento una propiedad nueva de ADO.NET(DATAROW)lista de datos laborales del empleado </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>concluido</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -525,6 +609,13 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -540,7 +631,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -548,11 +639,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -644,14 +744,28 @@
     <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="14">
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -659,9 +773,45 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Arial"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -693,6 +843,20 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -763,7 +927,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla3" displayName="Tabla3" ref="A10:H27" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla3" displayName="Tabla3" ref="A10:H27" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="A10:H27" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="LUNES"/>
@@ -780,12 +944,29 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{029EC875-0605-4C50-8F29-0FD4916AB6A8}" name="Tabla4" displayName="Tabla4" ref="A9:H11" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="8" tableBorderDxfId="9">
+  <autoFilter ref="A9:H11" xr:uid="{6983508E-6B95-42B3-BE2C-66A2E36269BB}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{4643AB56-0BAB-48FC-8306-468D1062DE86}" name="LUNES" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{E953D8AE-BD07-4A44-B608-F783C68D65C4}" name="MARTES" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{9FEC44C2-4D5F-4D3D-9CEE-CDD42DED5F8D}" name="MIÉRCOLES" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{48499542-CA4A-4882-A6B4-951C92C7BB31}" name="JUEVES" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{747A39BA-EC58-4CBC-929B-AC087F8AC0BB}" name="VIERNES" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{46E2C91C-9A07-4E58-BF2E-EFE1A87E5BFE}" name="SÁBADO" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{B8BDDE1B-47E6-4651-A198-53F748E08E3F}" name="DOMINGO" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{C51D3758-B97A-4E03-B404-E72F7D39CC77}" name="DEVELOPER"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabla1" displayName="Tabla1" ref="A2:D29" totalsRowShown="0">
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="OBSERVACION"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="PENDIENTE" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="CONCLUIDO" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="ENCARGADO" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="PENDIENTE" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="CONCLUIDO" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="ENCARGADO" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1090,8 +1271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:H27"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A26" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A25" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1516,11 +1697,128 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE52260-A7A4-4760-815C-05D6289EA23F}">
+  <dimension ref="A2:H11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="7" width="19.85546875" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="35" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="37">
+        <v>44074</v>
+      </c>
+      <c r="B10" s="37">
+        <v>44075</v>
+      </c>
+      <c r="C10" s="37">
+        <v>44076</v>
+      </c>
+      <c r="D10" s="37">
+        <v>44077</v>
+      </c>
+      <c r="E10" s="37">
+        <v>44078</v>
+      </c>
+      <c r="F10" s="37">
+        <v>44079</v>
+      </c>
+      <c r="G10" s="37">
+        <v>44080</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="195" x14ac:dyDescent="0.25">
+      <c r="A11" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" s="38" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="53" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A19" zoomScale="145" zoomScaleNormal="100" zoomScaleSheetLayoutView="145" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A19" zoomScale="145" zoomScaleNormal="100" zoomScaleSheetLayoutView="145" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1854,7 +2152,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
se corrigio error de fucion e informe actualizado
</commit_message>
<xml_diff>
--- a/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
+++ b/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
@@ -5,20 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mramirez\source\repos\PLANILLACONTABLE\INFORME\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462772C9-BAF2-48B3-88C2-80B812BEAED2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{885C4513-FA3E-4D72-81C6-984BB910A42A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="726" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="726" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="INFORME" sheetId="4" r:id="rId1"/>
-    <sheet name="PENDIENTES" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja1" sheetId="3" r:id="rId3"/>
+    <sheet name="INFORME AGOSTO" sheetId="4" r:id="rId1"/>
+    <sheet name="INFORME SEPTIEMBRE" sheetId="5" r:id="rId2"/>
+    <sheet name="PENDIENTES" sheetId="2" r:id="rId3"/>
+    <sheet name="PATRON" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">INFORME!$A$1:$H$27</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'INFORME AGOSTO'!$A$1:$H$27</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="96">
   <si>
     <t>INFORME DE  DESARROLLO DE SITEMA PLANILLA LCT.</t>
   </si>
@@ -400,12 +401,95 @@
   <si>
     <t>Modificar Procedimiento mostrar en sqlserver(banco, tipo documento, cargo, tipo de contrato) se borro varias lineas de codigo en sqlserver y C#</t>
   </si>
+  <si>
+    <t>Se inserto datos a la tabla Empleado y contrato (con un solo proceso)para eso, se modifico los procedimientos en SQLSERVER Y el codigo fuente en VBC#</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Listar solo Nombre de empleado al ser registrado y contratado, luego se tendra que mostrar todos sus datos laborales en los campos del formulario para su respectiva Actualizacion( </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pendiente</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>en</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pruebas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Se hizo varias pruebas(para mostrar datos laborales en campos del formulario), en conclucion se implemento una propiedad nueva de ADO.NET(DATAROW)lista de datos laborales del empleado </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>concluido</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -525,6 +609,13 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -540,7 +631,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -548,11 +639,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -644,11 +744,24 @@
     <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="14">
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -679,6 +792,60 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -763,7 +930,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla3" displayName="Tabla3" ref="A10:H27" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla3" displayName="Tabla3" ref="A10:H27" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="A10:H27" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="LUNES"/>
@@ -780,6 +947,23 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{029EC875-0605-4C50-8F29-0FD4916AB6A8}" name="Tabla4" displayName="Tabla4" ref="A9:H11" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10">
+  <autoFilter ref="A9:H11" xr:uid="{6983508E-6B95-42B3-BE2C-66A2E36269BB}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{4643AB56-0BAB-48FC-8306-468D1062DE86}" name="LUNES" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{E953D8AE-BD07-4A44-B608-F783C68D65C4}" name="MARTES" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{9FEC44C2-4D5F-4D3D-9CEE-CDD42DED5F8D}" name="MIÉRCOLES" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{48499542-CA4A-4882-A6B4-951C92C7BB31}" name="JUEVES" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{747A39BA-EC58-4CBC-929B-AC087F8AC0BB}" name="VIERNES" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{46E2C91C-9A07-4E58-BF2E-EFE1A87E5BFE}" name="SÁBADO" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{B8BDDE1B-47E6-4651-A198-53F748E08E3F}" name="DOMINGO" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{C51D3758-B97A-4E03-B404-E72F7D39CC77}" name="DEVELOPER"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabla1" displayName="Tabla1" ref="A2:D29" totalsRowShown="0">
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="OBSERVACION"/>
@@ -1090,8 +1274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:H27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A24" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A25" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1516,11 +1700,131 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE52260-A7A4-4760-815C-05D6289EA23F}">
+  <dimension ref="A2:H11"/>
+  <sheetViews>
+    <sheetView view="pageBreakPreview" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="7" width="19.85546875" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="35" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="37">
+        <v>44074</v>
+      </c>
+      <c r="B10" s="37">
+        <v>44075</v>
+      </c>
+      <c r="C10" s="37">
+        <v>44076</v>
+      </c>
+      <c r="D10" s="37">
+        <v>44077</v>
+      </c>
+      <c r="E10" s="37">
+        <v>44078</v>
+      </c>
+      <c r="F10" s="37">
+        <v>44079</v>
+      </c>
+      <c r="G10" s="37">
+        <v>44080</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="195" x14ac:dyDescent="0.25">
+      <c r="A11" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" s="38" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="39" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="53" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:E29"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" topLeftCell="A19" zoomScale="145" zoomScaleNormal="100" zoomScaleSheetLayoutView="145" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1854,15 +2158,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
se recupero de sqlserver idperiodo en form login
</commit_message>
<xml_diff>
--- a/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
+++ b/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\source\repos\lctsistemas\PLANILLACONTABLE\INFORME\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{885C4513-FA3E-4D72-81C6-984BB910A42A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F4CE11-7C0B-41E2-AD3D-35871D938930}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="726" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="726" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INFORME AGOSTO" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="97">
   <si>
     <t>INFORME DE  DESARROLLO DE SITEMA PLANILLA LCT.</t>
   </si>
@@ -483,6 +483,9 @@
       </rPr>
       <t>concluido</t>
     </r>
+  </si>
+  <si>
+    <t>Recuperacion  codigo idperiodo(de tabla pariodo en sqlserver)para el inicio de sesion y sus respectivas operaciones con el registro</t>
   </si>
 </sst>
 </file>
@@ -1703,8 +1706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE52260-A7A4-4760-815C-05D6289EA23F}">
   <dimension ref="A2:H11"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1802,7 +1805,9 @@
       <c r="C11" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="D11" s="36"/>
+      <c r="D11" s="38" t="s">
+        <v>96</v>
+      </c>
       <c r="E11" s="36"/>
       <c r="F11" s="36"/>
       <c r="G11" s="36"/>
@@ -2162,7 +2167,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
empleado y contrado modifica ok
</commit_message>
<xml_diff>
--- a/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
+++ b/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\source\repos\lctsistemas\PLANILLACONTABLE\INFORME\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F4CE11-7C0B-41E2-AD3D-35871D938930}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9568D454-238E-41BF-85B8-387144C96F36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="726" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="99">
   <si>
     <t>INFORME DE  DESARROLLO DE SITEMA PLANILLA LCT.</t>
   </si>
@@ -485,7 +485,13 @@
     </r>
   </si>
   <si>
-    <t>Recuperacion  codigo idperiodo(de tabla pariodo en sqlserver)para el inicio de sesion y sus respectivas operaciones con el registro</t>
+    <t xml:space="preserve">Procedimiento Modificar en sqlserver(empleado y contrato)y el codigo fuente en C# </t>
+  </si>
+  <si>
+    <t>Recuperacion  codigo idperiodo(de tabla periodo en sqlserver)para el inicio de sesion y sus respectivas operaciones con el registro</t>
+  </si>
+  <si>
+    <t>Analisis de Errores y corregidos</t>
   </si>
 </sst>
 </file>
@@ -1706,8 +1712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE52260-A7A4-4760-815C-05D6289EA23F}">
   <dimension ref="A2:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1806,10 +1812,14 @@
         <v>95</v>
       </c>
       <c r="D11" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="F11" s="38" t="s">
+        <v>98</v>
+      </c>
       <c r="G11" s="36"/>
       <c r="H11" s="39" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Implementar ApiRest consulta DNI
</commit_message>
<xml_diff>
--- a/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
+++ b/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\source\repos\lctsistemas\PLANILLACONTABLE\INFORME\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BFCB94-CFE1-4FA3-B349-6C61D7A83515}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8CAB922-4076-4A88-BC55-9CD215CCB75B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="726" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3015" yWindow="1350" windowWidth="15375" windowHeight="9720" tabRatio="726" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INFORME AGOSTO" sheetId="4" r:id="rId1"/>
@@ -1742,7 +1742,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE52260-A7A4-4760-815C-05D6289EA23F}">
   <dimension ref="A2:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
afp comisiones insertar masivo
</commit_message>
<xml_diff>
--- a/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
+++ b/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mramirez\source\repos\PLANILLACONTABLE\INFORME\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\source\repos\PLANILLACONTABLE\INFORME\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9AFE4F-AAC2-4D0A-9132-A01A0A13F06C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DAC1603-0CF4-478E-9F4B-708397D76BC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="726" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="726" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INFORME AGOSTO" sheetId="4" r:id="rId1"/>
@@ -997,25 +997,25 @@
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -1906,8 +1906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE52260-A7A4-4760-815C-05D6289EA23F}">
   <dimension ref="A2:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A14" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A17" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
informe de 5-10 al 10-10-20
</commit_message>
<xml_diff>
--- a/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
+++ b/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\source\repos\PLANILLACONTABLE\INFORME\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43248E23-2FB5-4DA5-8A04-5F7AC75C6662}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765C181E-36C3-4225-9AED-DBEDA5F903F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="726" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="144">
   <si>
     <t>INFORME DE  DESARROLLO DE SITEMA PLANILLA LCT.</t>
   </si>
@@ -752,6 +752,24 @@
   </si>
   <si>
     <t>Implementar Metodo y validaciones para la las horas extras, (horas extras  diurnas y  nocturnas)ok.</t>
+  </si>
+  <si>
+    <t>Calculo total horas extras, total remuneracion, feriados.</t>
+  </si>
+  <si>
+    <t>Validacion de calculo, y Tardanzas.</t>
+  </si>
+  <si>
+    <t>sin luz</t>
+  </si>
+  <si>
+    <t>Revision y Modificacion</t>
+  </si>
+  <si>
+    <t>Implementar algoritmo para insertar y modificar de forma masiva</t>
+  </si>
+  <si>
+    <t>Implementar algoritmo para insertar y modificar de forma masiva (OK), pero falta pruebas.</t>
   </si>
 </sst>
 </file>
@@ -876,6 +894,7 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -916,6 +935,7 @@
       <sz val="11"/>
       <color theme="4" tint="-0.249977111117893"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -954,7 +974,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1082,66 +1102,15 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="24">
-    <dxf>
-      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1172,6 +1141,60 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
@@ -1344,16 +1367,16 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{64C7FF56-F474-4584-B1AB-2005F0AD6B48}" name="Tabla43" displayName="Tabla43" ref="A9:H21" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="7" tableBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{64C7FF56-F474-4584-B1AB-2005F0AD6B48}" name="Tabla43" displayName="Tabla43" ref="A9:H21" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10">
   <autoFilter ref="A9:H21" xr:uid="{6983508E-6B95-42B3-BE2C-66A2E36269BB}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{DE1C6334-763D-4EFD-820F-8338CCB0D61A}" name="LUNES" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{CFA4FF71-F041-49B1-B161-9FF49BEC461C}" name="MARTES" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{8CC4D981-27D4-4E4F-9AC3-11CB7C096EEF}" name="MIÉRCOLES" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{BA7535F5-C99F-4699-9028-08DC89F6C4B9}" name="JUEVES" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{037149CF-875B-4884-80F5-8D6756F292C9}" name="VIERNES" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{E1786BD5-7D4B-4CC1-9CF9-55A6890ED160}" name="SÁBADO" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{415CB197-C16B-4996-912D-D31D3D9A21E0}" name="DOMINGO" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{DE1C6334-763D-4EFD-820F-8338CCB0D61A}" name="LUNES" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{CFA4FF71-F041-49B1-B161-9FF49BEC461C}" name="MARTES" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{8CC4D981-27D4-4E4F-9AC3-11CB7C096EEF}" name="MIÉRCOLES" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{BA7535F5-C99F-4699-9028-08DC89F6C4B9}" name="JUEVES" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{037149CF-875B-4884-80F5-8D6756F292C9}" name="VIERNES" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{E1786BD5-7D4B-4CC1-9CF9-55A6890ED160}" name="SÁBADO" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{415CB197-C16B-4996-912D-D31D3D9A21E0}" name="DOMINGO" dataDxfId="3"/>
     <tableColumn id="8" xr3:uid="{83EDBEE9-3894-4F87-A0C6-238778E933C3}" name="DEVELOPER"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1364,9 +1387,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabla1" displayName="Tabla1" ref="A2:D31" totalsRowShown="0">
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="OBSERVACION"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="PENDIENTE" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="CONCLUIDO" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="ENCARGADO" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="PENDIENTE" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="CONCLUIDO" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="ENCARGADO" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2462,8 +2485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF054BD2-E95A-4F49-B047-EB049B2379A9}">
   <dimension ref="A2:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2596,15 +2619,29 @@
         <v>44115</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="38"/>
-      <c r="B13" s="38"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
+    <row r="13" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="B13" s="38" t="s">
+        <v>139</v>
+      </c>
+      <c r="C13" s="50" t="s">
+        <v>140</v>
+      </c>
+      <c r="D13" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="E13" s="38" t="s">
+        <v>142</v>
+      </c>
+      <c r="F13" s="38" t="s">
+        <v>143</v>
+      </c>
       <c r="G13" s="36"/>
-      <c r="H13" s="39"/>
+      <c r="H13" s="17" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="37"/>

</xml_diff>

<commit_message>
Informe del 12-10-2020 al 17-10-20
</commit_message>
<xml_diff>
--- a/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
+++ b/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\source\repos\PLANILLACONTABLE\INFORME\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765C181E-36C3-4225-9AED-DBEDA5F903F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08345828-79B9-4A2E-9BCD-596DD9139169}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="726" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="149">
   <si>
     <t>INFORME DE  DESARROLLO DE SITEMA PLANILLA LCT.</t>
   </si>
@@ -770,6 +770,21 @@
   </si>
   <si>
     <t>Implementar algoritmo para insertar y modificar de forma masiva (OK), pero falta pruebas.</t>
+  </si>
+  <si>
+    <t>Pruebas en Insercion Masiva en C#</t>
+  </si>
+  <si>
+    <t>Coordinar Cuadro Subsidios, detalles.</t>
+  </si>
+  <si>
+    <t>Funciones y condiciones para el calculo de la planilla En C#), se esta validando por empleado el Subsidio</t>
+  </si>
+  <si>
+    <t>Validaciones Pendientes, hay Errores.</t>
+  </si>
+  <si>
+    <t>Se creo otro formulario en C# de  Subsidio, para no alterar el que ya estaba creado con modificaciones, y se implemento algoritmo Pruebas inserción masiva y modificación masiva  (en formulario AFP) Funciono Correctamente. Lo mismo se insertara para registrar el calculo de la planilla mensual.</t>
   </si>
 </sst>
 </file>
@@ -2485,8 +2500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF054BD2-E95A-4F49-B047-EB049B2379A9}">
   <dimension ref="A2:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A14" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2594,7 +2609,9 @@
         <v>137</v>
       </c>
       <c r="G11" s="40"/>
-      <c r="H11" s="42"/>
+      <c r="H11" s="42" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="37">
@@ -2644,24 +2661,50 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="37"/>
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
+      <c r="A14" s="37">
+        <v>44116</v>
+      </c>
+      <c r="B14" s="37">
+        <v>44117</v>
+      </c>
+      <c r="C14" s="37">
+        <v>44118</v>
+      </c>
+      <c r="D14" s="37">
+        <v>44119</v>
+      </c>
+      <c r="E14" s="37">
+        <v>44120</v>
+      </c>
+      <c r="F14" s="37">
+        <v>44121</v>
+      </c>
+      <c r="G14" s="37">
+        <v>44122</v>
+      </c>
       <c r="H14" s="39"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="38"/>
-      <c r="B15" s="38"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
+    <row r="15" spans="1:8" ht="255" x14ac:dyDescent="0.25">
+      <c r="A15" s="38" t="s">
+        <v>144</v>
+      </c>
+      <c r="B15" s="38" t="s">
+        <v>145</v>
+      </c>
+      <c r="C15" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="D15" s="38" t="s">
+        <v>147</v>
+      </c>
+      <c r="E15" s="38" t="s">
+        <v>148</v>
+      </c>
       <c r="F15" s="38"/>
       <c r="G15" s="38"/>
-      <c r="H15" s="1"/>
+      <c r="H15" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="37"/>

</xml_diff>

<commit_message>
informe 19-10-20 al 24-10-2020
</commit_message>
<xml_diff>
--- a/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
+++ b/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\source\repos\PLANILLACONTABLE\INFORME\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC7319A-B44C-4CDF-AF3C-5EF97D516E0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD02241B-83BD-40D2-9CC8-3069B9212A5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="726" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="155">
   <si>
     <t>INFORME DE  DESARROLLO DE SITEMA PLANILLA LCT.</t>
   </si>
@@ -785,6 +785,24 @@
   </si>
   <si>
     <t>Se creo otro formulario en C# de  Subsidio, para no alterar el que ya estaba creado con modificaciones, y se implemento algoritmo Pruebas inserción masiva y modificación masiva  (en formulario AFP) Funciono Correctamente. Lo mismo se insertara para registrar el calculo de la planilla mensual.</t>
+  </si>
+  <si>
+    <t>Tabla subsidos y detalle, en sqlserver(script de procedimientos (sp)para el mantenimiento)</t>
+  </si>
+  <si>
+    <t>Metodos de acceso(capa datos y negocio) metodos en C# para mantenimiento de subsidios</t>
+  </si>
+  <si>
+    <t>Formulario Calculo planilla(validar dias subsidiados y aplicar formula para el calculo)</t>
+  </si>
+  <si>
+    <t>Validacion subsidiados y no subsidiados en formulario calculo de planilla (mostrar datos según el tipo) en C#</t>
+  </si>
+  <si>
+    <t>Formulario subsidio(agregar, modificar y eliminar) sumas de dias subsidiados por tipo. En C#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se valido codigo subsidios(supension perfecta y suspension imperfecta) para mostrar los dias en casillas de formulario calculo planilla) </t>
   </si>
 </sst>
 </file>
@@ -2501,7 +2519,7 @@
   <dimension ref="A2:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A14" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2707,32 +2725,75 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="37"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="41"/>
-      <c r="B17" s="41"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="40"/>
+      <c r="A16" s="37">
+        <v>44123</v>
+      </c>
+      <c r="B16" s="37">
+        <v>44124</v>
+      </c>
+      <c r="C16" s="37">
+        <v>44125</v>
+      </c>
+      <c r="D16" s="37">
+        <v>44126</v>
+      </c>
+      <c r="E16" s="37">
+        <v>44127</v>
+      </c>
+      <c r="F16" s="37">
+        <v>44128</v>
+      </c>
+      <c r="G16" s="37">
+        <v>44129</v>
+      </c>
+      <c r="H16" s="39"/>
+    </row>
+    <row r="17" spans="1:8" ht="128.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="41" t="s">
+        <v>149</v>
+      </c>
+      <c r="B17" s="41" t="s">
+        <v>150</v>
+      </c>
+      <c r="C17" s="41" t="s">
+        <v>152</v>
+      </c>
+      <c r="D17" s="41" t="s">
+        <v>153</v>
+      </c>
+      <c r="E17" s="41" t="s">
+        <v>151</v>
+      </c>
+      <c r="F17" s="41" t="s">
+        <v>154</v>
+      </c>
       <c r="G17" s="40"/>
-      <c r="H17" s="42"/>
+      <c r="H17" s="42" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="43"/>
-      <c r="B18" s="43"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
+      <c r="A18" s="43">
+        <v>44130</v>
+      </c>
+      <c r="B18" s="43">
+        <v>44131</v>
+      </c>
+      <c r="C18" s="43">
+        <v>44132</v>
+      </c>
+      <c r="D18" s="43">
+        <v>44133</v>
+      </c>
+      <c r="E18" s="43">
+        <v>44134</v>
+      </c>
+      <c r="F18" s="43">
+        <v>44135</v>
+      </c>
+      <c r="G18" s="43">
+        <v>44136</v>
+      </c>
       <c r="H18" s="44"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -3146,7 +3207,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
informe del 26-10-2020 al 31-10-2020
</commit_message>
<xml_diff>
--- a/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
+++ b/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\source\repos\PLANILLACONTABLE\INFORME\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B0E530-62C1-41F6-829D-3C89713B5989}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{962C8A28-F78F-4CC4-9417-A387033E6AFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="726" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="165">
   <si>
     <t>INFORME DE  DESARROLLO DE SITEMA PLANILLA LCT.</t>
   </si>
@@ -827,6 +827,12 @@
   </si>
   <si>
     <t xml:space="preserve">Se implemento en el formulario calculo(codigo contrato, codigo planilla, dias dominicales y horas diarias trabajadas) se valido para que ingrese dias y calcule las horas diarias trabajas </t>
+  </si>
+  <si>
+    <t>Se creo tabla planilla y todos sus atributos en LA BASE DE DATOS</t>
+  </si>
+  <si>
+    <t>Algoritmo para Recuperar Registro de planilla y Mostrar en el formulario planilla calculo validando los  numeros ceros con null.</t>
   </si>
 </sst>
 </file>
@@ -1031,7 +1037,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1162,6 +1168,9 @@
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2543,7 +2552,7 @@
   <dimension ref="A2:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A18" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2877,10 +2886,16 @@
       <c r="D21" s="47" t="s">
         <v>162</v>
       </c>
-      <c r="E21" s="48"/>
-      <c r="F21" s="47"/>
+      <c r="E21" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="F21" s="38" t="s">
+        <v>164</v>
+      </c>
       <c r="G21" s="48"/>
-      <c r="H21" s="33"/>
+      <c r="H21" s="51" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="43"/>

</xml_diff>

<commit_message>
informe de 02-11-2020 al 07-11-2020
</commit_message>
<xml_diff>
--- a/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
+++ b/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mramirez\source\repos\PLANILLACONTABLE\INFORME\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\source\repos\PLANILLACONTABLE\INFORME\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C381A8-8B35-4B18-9BA8-9F5184AEB412}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E263007B-A7BA-4BFD-8C9D-230FFDA7D677}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="726" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="726" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INFORME AGOSTO" sheetId="4" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="172">
   <si>
     <t>INFORME DE  DESARROLLO DE SITEMA PLANILLA LCT.</t>
   </si>
@@ -843,14 +843,23 @@
   <si>
     <t>creacion de procedimientos almacenados para el mantenimienot de subsidios.</t>
   </si>
+  <si>
+    <t xml:space="preserve">Formulario Calculo( metodos para mostrar empleados ), modificacion tablas en SQLSERVER y codigo en C#(tipo de documento, contrato, regimen salud) </t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Modificacion formulario calculo( diseño de agregar y quitar conceptos de la tabla calculo), Cambiar diseño  de calculo de planilla y inicio de sesion( según acordado)</t>
+  </si>
+  <si>
+    <t>diseño inicio de sesion y revision de codigo en SQLSERVER (se borro los procedimientos que ya no se usaran.(según acordado)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
-  </numFmts>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1049,7 +1058,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1184,7 +1193,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1222,25 +1234,25 @@
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -1276,25 +1288,25 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -1446,8 +1458,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{64C7FF56-F474-4584-B1AB-2005F0AD6B48}" name="Tabla43" displayName="Tabla43" ref="A9:H23" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10">
-  <autoFilter ref="A9:H23" xr:uid="{6983508E-6B95-42B3-BE2C-66A2E36269BB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{64C7FF56-F474-4584-B1AB-2005F0AD6B48}" name="Tabla43" displayName="Tabla43" ref="A9:H26" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10">
+  <autoFilter ref="A9:H26" xr:uid="{6983508E-6B95-42B3-BE2C-66A2E36269BB}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{DE1C6334-763D-4EFD-820F-8338CCB0D61A}" name="LUNES" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{CFA4FF71-F041-49B1-B161-9FF49BEC461C}" name="MARTES" dataDxfId="8"/>
@@ -2562,10 +2574,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF054BD2-E95A-4F49-B047-EB049B2379A9}">
-  <dimension ref="A2:H24"/>
+  <dimension ref="A2:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A20" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A23" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2953,14 +2965,59 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="47"/>
-      <c r="B24" s="47"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="47"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="47"/>
-      <c r="G24" s="48"/>
-      <c r="H24" s="33"/>
+      <c r="A24" s="43">
+        <v>44137</v>
+      </c>
+      <c r="B24" s="43">
+        <v>44138</v>
+      </c>
+      <c r="C24" s="43">
+        <v>44139</v>
+      </c>
+      <c r="D24" s="43">
+        <v>44140</v>
+      </c>
+      <c r="E24" s="43">
+        <v>44141</v>
+      </c>
+      <c r="F24" s="43">
+        <v>44142</v>
+      </c>
+      <c r="G24" s="43">
+        <v>44143</v>
+      </c>
+      <c r="H24" s="44"/>
+    </row>
+    <row r="25" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+      <c r="A25" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="B25" s="52"/>
+      <c r="C25" s="52" t="s">
+        <v>169</v>
+      </c>
+      <c r="D25" s="52" t="s">
+        <v>169</v>
+      </c>
+      <c r="E25" s="38" t="s">
+        <v>170</v>
+      </c>
+      <c r="F25" s="38" t="s">
+        <v>171</v>
+      </c>
+      <c r="G25" s="52"/>
+      <c r="H25" s="53" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="52"/>
+      <c r="B26" s="52"/>
+      <c r="C26" s="52"/>
+      <c r="D26" s="52"/>
+      <c r="E26" s="52"/>
+      <c r="F26" s="52"/>
+      <c r="G26" s="52"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
informe del 9-11-2020 al 14-11-2020
</commit_message>
<xml_diff>
--- a/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
+++ b/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\source\repos\PLANILLACONTABLE\INFORME\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EDFEE32-BAC8-4563-B6D1-91C589B600D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A2701F-7885-41EC-842D-2531F16B2293}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="726" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2604,7 +2604,7 @@
   <dimension ref="A2:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A26" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
informe del 16-11-2020 al 21-11-2020
</commit_message>
<xml_diff>
--- a/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
+++ b/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mramirez\source\repos\PLANILLACONTABLE\INFORME\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB9E609-6CB6-4EAA-9F7D-5D9521D4B3D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C2FFCD-A349-4B0D-B001-A632B4E49CB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="726" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="726" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INFORME AGOSTO" sheetId="4" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="187">
   <si>
     <t>INFORME DE  DESARROLLO DE SITEMA PLANILLA LCT.</t>
   </si>
@@ -883,13 +883,34 @@
     <t>Dias Vacaciones (separar los dias con validaciones en tabla  no subsidios no laborados, para su calculo respectivo. Calculo montos por trabajador(ONP, Y COMISIONES, SEGUROS, APORTES  DE AFP)</t>
   </si>
   <si>
-    <t>Verificacion de errores en los formulario cargo, empresa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modificacion de los procedimientos almacenados para optimizar el registro y mantenimiento. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Formulario de subsidios completo con registro, modificacion y eliminacion. </t>
+    <t>Validar los controles  CHECKBOX para al hacer cuando hacemos click  ocultemos  los campos de la planilla, metodo para cada campo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Procedimiento almacenado Registrar o Actualizar segun caso en SQL, Metodos set and get en C# para comunicar los parametros, clases(Dconcepto, Rconcepto, Nconcepto) </t>
+  </si>
+  <si>
+    <t>nombre a los Controles CHECKBOX, para su validacion  con diseño completado</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Procedo registrar y pruebas tabla Conceptos en C#, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>error faltal al sincronizar  en el proyecto(se tuvo que hacer los cambios ya avazados desde el lunes</t>
+    </r>
+  </si>
+  <si>
+    <t>se modifico algoritmo calculo(ya que fue alterado al agreagar nuevos campos a la planilla), se agrego los nuevos campos a la tabla en la Base de datos. Se calculo aporte a O.N.P Y A.F.P , por cada trabajador</t>
+  </si>
+  <si>
+    <t>formulario crear planilla y planilla calculo(se unieron y muestra los datos necesarios al seleccionar por periodo ok.</t>
   </si>
 </sst>
 </file>
@@ -1270,25 +1291,25 @@
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -1324,25 +1345,25 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -2610,16 +2631,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF054BD2-E95A-4F49-B047-EB049B2379A9}">
-  <dimension ref="A2:H32"/>
+  <dimension ref="A2:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A26" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A30" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="7" width="19.85546875" customWidth="1"/>
-    <col min="8" max="8" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -3114,83 +3135,77 @@
       </c>
       <c r="H28" s="44"/>
     </row>
-    <row r="29" spans="1:8" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A29" s="38" t="s">
         <v>175</v>
       </c>
       <c r="B29" s="38" t="s">
-        <v>181</v>
-      </c>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
+        <v>176</v>
+      </c>
+      <c r="C29" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="D29" s="38" t="s">
+        <v>178</v>
+      </c>
       <c r="E29" s="38" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F29" s="38" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G29" s="52"/>
       <c r="H29" s="17" t="s">
-        <v>155</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="43">
-        <v>44144</v>
+        <v>44151</v>
       </c>
       <c r="B30" s="43">
-        <v>44145</v>
+        <v>44152</v>
       </c>
       <c r="C30" s="43">
-        <v>44146</v>
+        <v>44153</v>
       </c>
       <c r="D30" s="43">
-        <v>44147</v>
+        <v>44154</v>
       </c>
       <c r="E30" s="43">
-        <v>44148</v>
+        <v>44155</v>
       </c>
       <c r="F30" s="43">
-        <v>44149</v>
+        <v>44156</v>
       </c>
       <c r="G30" s="43">
-        <v>44150</v>
+        <v>44157</v>
       </c>
       <c r="H30" s="44"/>
     </row>
     <row r="31" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A31" s="38" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="B31" s="38" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="C31" s="38" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="D31" s="38" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="E31" s="38" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="F31" s="38" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="G31" s="52"/>
       <c r="H31" s="17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="38"/>
-      <c r="B32" s="38"/>
-      <c r="C32" s="38"/>
-      <c r="D32" s="38"/>
-      <c r="E32" s="38"/>
-      <c r="F32" s="38"/>
-      <c r="G32" s="52"/>
-      <c r="H32" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
empleado y contrato modificaciones add jornada laboral
</commit_message>
<xml_diff>
--- a/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
+++ b/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mramirez\source\repos\PLANILLACONTABLE\INFORME\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\source\repos\PLANILLACONTABLE\INFORME\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2678C4B3-FD33-4978-B4EA-1BC7286F1F3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D9073A-EF86-416D-B775-BFF26CE61F81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" tabRatio="726" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="726" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INFORME AGOSTO" sheetId="4" r:id="rId1"/>
@@ -929,9 +929,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
-  </numFmts>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1269,7 +1266,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1309,25 +1306,25 @@
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -1363,25 +1360,25 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -2652,7 +2649,7 @@
   <dimension ref="A2:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A30" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3218,7 +3215,7 @@
       </c>
       <c r="G31" s="52"/>
       <c r="H31" s="17" t="s">
-        <v>15</v>
+        <v>155</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -3266,7 +3263,7 @@
       </c>
       <c r="G33" s="52"/>
       <c r="H33" s="17" t="s">
-        <v>155</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
inicio de sesion terminado unido con frmprincipal
</commit_message>
<xml_diff>
--- a/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
+++ b/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\source\repos\PLANILLACONTABLE\INFORME\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A5614E-1124-4DCC-A702-5DE385E68797}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F12CE8-8408-4221-B77D-FB171CF9E2E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="726" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="197">
   <si>
     <t>INFORME DE  DESARROLLO DE SITEMA PLANILLA LCT.</t>
   </si>
@@ -926,6 +926,44 @@
   </si>
   <si>
     <t>Modificacion a empleado se agrego Jornada laboral(part-time y full-time), en C# y SQL, se creo procedimiento ANULAR empleado con validacion(en SQL Y c#).</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">En formulario crear planilla se implento codigo (validar meses repetidos), se cambio todo el diseño de inicio de sesion(se agrego ROL para ser validado, y se modifico el procedimiento en SQL que hace referencia al LOGIN, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>aun falta codigo para iniciar sesion</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <t>Planilla de calculo(se agrego un campo para poder validar el Part - Time, cambio en el procedimiento de SQL SERVER</t>
+  </si>
+  <si>
+    <t>se finalizo el diseño de INICIO DE SESION por ende se  cambio de todo el codigo para el inicio de sesion, agregando nuevos datos  a mostrar.</t>
+  </si>
+  <si>
+    <t>Revision de los formulario auxiliares para el registro de empleado(se corrigio tanto la vista como el codigo fuente)</t>
+  </si>
+  <si>
+    <t>En empleado se implemento codigo para validar (codigo dni-independiente para otras empresas)</t>
   </si>
 </sst>
 </file>
@@ -2651,8 +2689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF054BD2-E95A-4F49-B047-EB049B2379A9}">
   <dimension ref="A2:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A33" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A34" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3293,17 +3331,27 @@
       </c>
       <c r="H34" s="44"/>
     </row>
-    <row r="35" spans="1:8" ht="135" x14ac:dyDescent="0.25">
-      <c r="A35" s="52"/>
-      <c r="B35" s="52"/>
+    <row r="35" spans="1:8" ht="210" x14ac:dyDescent="0.25">
+      <c r="A35" s="54" t="s">
+        <v>191</v>
+      </c>
+      <c r="B35" s="54" t="s">
+        <v>195</v>
+      </c>
       <c r="C35" s="54" t="s">
-        <v>191</v>
-      </c>
-      <c r="D35" s="52"/>
-      <c r="E35" s="52"/>
-      <c r="F35" s="52"/>
+        <v>196</v>
+      </c>
+      <c r="D35" s="54" t="s">
+        <v>192</v>
+      </c>
+      <c r="E35" s="54" t="s">
+        <v>193</v>
+      </c>
+      <c r="F35" s="54" t="s">
+        <v>194</v>
+      </c>
       <c r="G35" s="52"/>
-      <c r="H35" t="s">
+      <c r="H35" s="9" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modificaciones en codigo de presentacion y index de calculo ordenado
</commit_message>
<xml_diff>
--- a/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
+++ b/INFORME/INFORME PLANILLA CONTABLE 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\source\repos\PLANILLACONTABLE\INFORME\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8C7EE8-8A18-40CB-AC76-6477D28CAAF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19806DC2-88D3-4B4B-8A91-CB044A38F7C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="726" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="215">
   <si>
     <t>INFORME DE  DESARROLLO DE SITEMA PLANILLA LCT.</t>
   </si>
@@ -1053,12 +1053,21 @@
       <t>) para el calculo. Los PART - TIME (seran otro color de letra para distinguir)</t>
     </r>
   </si>
+  <si>
+    <t>se organizo el menu principal, y se configuro el acceso por Roles de Usuario</t>
+  </si>
+  <si>
+    <t>Modificaciones en Formularios pendientes</t>
+  </si>
+  <si>
+    <t>Modificaciones en formulario(Banco)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1225,13 +1234,6 @@
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -3550,7 +3552,7 @@
   <dimension ref="A2:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3705,7 +3707,9 @@
         <v>205</v>
       </c>
       <c r="G13" s="52"/>
-      <c r="H13" s="17"/>
+      <c r="H13" s="17" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="37">
@@ -3751,27 +3755,53 @@
         <v>211</v>
       </c>
       <c r="G15" s="54"/>
-      <c r="H15" s="9"/>
+      <c r="H15" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="37"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
+      <c r="A16" s="37">
+        <v>44186</v>
+      </c>
+      <c r="B16" s="37">
+        <v>44187</v>
+      </c>
+      <c r="C16" s="37">
+        <v>44188</v>
+      </c>
+      <c r="D16" s="37">
+        <v>44189</v>
+      </c>
+      <c r="E16" s="37">
+        <v>44190</v>
+      </c>
+      <c r="F16" s="37">
+        <v>44191</v>
+      </c>
+      <c r="G16" s="37">
+        <v>44192</v>
+      </c>
       <c r="H16" s="39"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A17" s="41"/>
-      <c r="B17" s="41"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
+      <c r="B17" s="41" t="s">
+        <v>212</v>
+      </c>
+      <c r="C17" s="41" t="s">
+        <v>213</v>
+      </c>
+      <c r="D17" s="41" t="s">
+        <v>169</v>
+      </c>
+      <c r="E17" s="41" t="s">
+        <v>214</v>
+      </c>
       <c r="F17" s="41"/>
       <c r="G17" s="40"/>
-      <c r="H17" s="42"/>
+      <c r="H17" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="37"/>

</xml_diff>